<commit_message>
test search and sorting  documented
</commit_message>
<xml_diff>
--- a/com.verizon/src/test/resources/test_data.xlsx
+++ b/com.verizon/src/test/resources/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadou\IdeaProjects\SeleniumBootcamp\com.verizon\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FDBC40B-91C9-446E-93E5-EB2826A28310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3559D1B3-B851-4A07-AB2B-AC89BECC0670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B5AA5C7D-1AF8-47EC-B017-3C6366FC6D0C}"/>
   </bookViews>
@@ -400,7 +400,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
test find stores in progress
</commit_message>
<xml_diff>
--- a/com.verizon/src/test/resources/test_data.xlsx
+++ b/com.verizon/src/test/resources/test_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadou\IdeaProjects\SeleniumBootcamp\com.verizon\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA5305B-6A64-4B90-82E4-A43E2A1AA727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF1C201-5694-423E-B373-ECB1DDAB4922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B5AA5C7D-1AF8-47EC-B017-3C6366FC6D0C}"/>
+    <workbookView xWindow="1608" yWindow="1332" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{B5AA5C7D-1AF8-47EC-B017-3C6366FC6D0C}"/>
   </bookViews>
   <sheets>
     <sheet name="doSearch" sheetId="1" r:id="rId1"/>
+    <sheet name="doFindStores" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Search Term</t>
   </si>
@@ -46,6 +47,9 @@
   </si>
   <si>
     <t>iphone 13</t>
+  </si>
+  <si>
+    <t>Zip Code</t>
   </si>
 </sst>
 </file>
@@ -399,7 +403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7698329-515D-4C3B-AE93-7DE2BD4AD69C}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -431,4 +435,47 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{534973A3-3AE8-4C30-B10A-5E2875B95CC7}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>19107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>19130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>19104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>19152</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
test add to favorite
</commit_message>
<xml_diff>
--- a/com.verizon/src/test/resources/test_data.xlsx
+++ b/com.verizon/src/test/resources/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadou\IdeaProjects\SeleniumBootcamp\com.verizon\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF1C201-5694-423E-B373-ECB1DDAB4922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095397FE-EC24-40CB-B5A6-EA3198194038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1608" yWindow="1332" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{B5AA5C7D-1AF8-47EC-B017-3C6366FC6D0C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Search Term</t>
   </si>
@@ -50,6 +50,18 @@
   </si>
   <si>
     <t>Zip Code</t>
+  </si>
+  <si>
+    <t>Philadelphia</t>
+  </si>
+  <si>
+    <t>New york</t>
+  </si>
+  <si>
+    <t>Washington D.C</t>
+  </si>
+  <si>
+    <t>Kenwood</t>
   </si>
 </sst>
 </file>
@@ -442,7 +454,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -456,23 +468,23 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>19107</v>
+      <c r="A2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>19130</v>
+      <c r="A3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>19104</v>
+      <c r="A4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>19152</v>
+      <c r="A5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>